<commit_message>
heapsort k4 Raspberry Pi measurements
This update contains: (1) k-analysis for Raspberry Pi that found that k=4 is optimal, (2) runtime log and siglent power and current measurements for heapsort k=4 running on Raspberry Pi
</commit_message>
<xml_diff>
--- a/Analysis/Raspberry Pi/analysis k time comparison.xlsx
+++ b/Analysis/Raspberry Pi/analysis k time comparison.xlsx
@@ -8,14 +8,59 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/majaht/github-directories/heap-sort/Analysis/Raspberry Pi/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{C530F8AD-4E05-F144-90A6-C7D10F1CCD35}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{58F96F4A-4BBF-A54C-BADD-BF2A64315A38}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="4300" yWindow="2700" windowWidth="27640" windowHeight="16940" xr2:uid="{C57EDD1A-ABCF-2D45-A5FE-2107AA50A042}"/>
+    <workbookView xWindow="5640" yWindow="2340" windowWidth="27640" windowHeight="16940" activeTab="1" xr2:uid="{C57EDD1A-ABCF-2D45-A5FE-2107AA50A042}"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Sheet2" sheetId="2" r:id="rId1"/>
+    <sheet name="Sheet1" sheetId="1" r:id="rId2"/>
   </sheets>
+  <definedNames>
+    <definedName name="_xlchart.v1.0" hidden="1">Sheet1!$B$1</definedName>
+    <definedName name="_xlchart.v1.1" hidden="1">Sheet1!$B$2:$B$44</definedName>
+    <definedName name="_xlchart.v1.10" hidden="1">Sheet1!$D$1</definedName>
+    <definedName name="_xlchart.v1.11" hidden="1">Sheet1!$D$2:$D$43</definedName>
+    <definedName name="_xlchart.v1.12" hidden="1">Sheet1!$B$1</definedName>
+    <definedName name="_xlchart.v1.13" hidden="1">Sheet1!$B$2:$B$44</definedName>
+    <definedName name="_xlchart.v1.14" hidden="1">Sheet1!$C$1</definedName>
+    <definedName name="_xlchart.v1.15" hidden="1">Sheet1!$C$2:$C$44</definedName>
+    <definedName name="_xlchart.v1.16" hidden="1">Sheet1!$D$1</definedName>
+    <definedName name="_xlchart.v1.17" hidden="1">Sheet1!$D$2:$D$44</definedName>
+    <definedName name="_xlchart.v1.18" hidden="1">Sheet1!$B$1</definedName>
+    <definedName name="_xlchart.v1.19" hidden="1">Sheet1!$B$2:$B$44</definedName>
+    <definedName name="_xlchart.v1.2" hidden="1">Sheet1!$C$1</definedName>
+    <definedName name="_xlchart.v1.20" hidden="1">Sheet1!$C$1</definedName>
+    <definedName name="_xlchart.v1.21" hidden="1">Sheet1!$C$2:$C$44</definedName>
+    <definedName name="_xlchart.v1.22" hidden="1">Sheet1!$D$1</definedName>
+    <definedName name="_xlchart.v1.23" hidden="1">Sheet1!$D$2:$D$44</definedName>
+    <definedName name="_xlchart.v1.24" hidden="1">Sheet1!$B$2:$B$9</definedName>
+    <definedName name="_xlchart.v1.25" hidden="1">Sheet1!$C$2:$C$9</definedName>
+    <definedName name="_xlchart.v1.26" hidden="1">Sheet1!$D$2:$D$9</definedName>
+    <definedName name="_xlchart.v1.27" hidden="1">Sheet1!$B$1</definedName>
+    <definedName name="_xlchart.v1.28" hidden="1">Sheet1!$B$2:$B$43</definedName>
+    <definedName name="_xlchart.v1.29" hidden="1">Sheet1!$C$1</definedName>
+    <definedName name="_xlchart.v1.3" hidden="1">Sheet1!$C$2:$C$44</definedName>
+    <definedName name="_xlchart.v1.30" hidden="1">Sheet1!$C$2:$C$43</definedName>
+    <definedName name="_xlchart.v1.31" hidden="1">Sheet1!$D$1</definedName>
+    <definedName name="_xlchart.v1.32" hidden="1">Sheet1!$D$2:$D$43</definedName>
+    <definedName name="_xlchart.v1.33" hidden="1">Sheet1!$B$1</definedName>
+    <definedName name="_xlchart.v1.34" hidden="1">Sheet1!$B$2:$B$44</definedName>
+    <definedName name="_xlchart.v1.35" hidden="1">Sheet1!$C$1</definedName>
+    <definedName name="_xlchart.v1.36" hidden="1">Sheet1!$C$2:$C$44</definedName>
+    <definedName name="_xlchart.v1.37" hidden="1">Sheet1!$D$1</definedName>
+    <definedName name="_xlchart.v1.38" hidden="1">Sheet1!$D$2:$D$44</definedName>
+    <definedName name="_xlchart.v1.4" hidden="1">Sheet1!$D$1</definedName>
+    <definedName name="_xlchart.v1.5" hidden="1">Sheet1!$D$2:$D$44</definedName>
+    <definedName name="_xlchart.v1.6" hidden="1">Sheet1!$B$1</definedName>
+    <definedName name="_xlchart.v1.7" hidden="1">Sheet1!$B$2:$B$43</definedName>
+    <definedName name="_xlchart.v1.8" hidden="1">Sheet1!$C$1</definedName>
+    <definedName name="_xlchart.v1.9" hidden="1">Sheet1!$C$2:$C$43</definedName>
+  </definedNames>
   <calcPr calcId="181029"/>
+  <pivotCaches>
+    <pivotCache cacheId="3" r:id="rId3"/>
+  </pivotCaches>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -36,7 +81,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="44" uniqueCount="44">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="50" uniqueCount="49">
   <si>
     <t>../../build/executables/N10240_K16.heapsort.out</t>
   </si>
@@ -168,6 +213,21 @@
   </si>
   <si>
     <t>N</t>
+  </si>
+  <si>
+    <t>tid</t>
+  </si>
+  <si>
+    <t>Sum of tid</t>
+  </si>
+  <si>
+    <t>Column Labels</t>
+  </si>
+  <si>
+    <t>Row Labels</t>
+  </si>
+  <si>
+    <t>Grand Total</t>
   </si>
 </sst>
 </file>
@@ -209,9 +269,14 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" pivotButton="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -227,6 +292,1698 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="en-GB"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-DK"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:scatterChart>
+        <c:scatterStyle val="lineMarker"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet1!$B$1</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>K</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="25400" cap="rnd">
+              <a:noFill/>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="lt1"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:yVal>
+            <c:numRef>
+              <c:f>Sheet1!$B$2:$B$44</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="43"/>
+                <c:pt idx="0">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>8</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>16</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>32</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>64</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>8</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>16</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>32</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>64</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>8</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>16</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>32</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>64</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>8</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>16</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>32</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>64</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>8</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>16</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>32</c:v>
+                </c:pt>
+                <c:pt idx="29">
+                  <c:v>64</c:v>
+                </c:pt>
+                <c:pt idx="30">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="31">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="32">
+                  <c:v>8</c:v>
+                </c:pt>
+                <c:pt idx="33">
+                  <c:v>16</c:v>
+                </c:pt>
+                <c:pt idx="34">
+                  <c:v>32</c:v>
+                </c:pt>
+                <c:pt idx="35">
+                  <c:v>64</c:v>
+                </c:pt>
+                <c:pt idx="36">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="37">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="38">
+                  <c:v>8</c:v>
+                </c:pt>
+                <c:pt idx="39">
+                  <c:v>16</c:v>
+                </c:pt>
+                <c:pt idx="40">
+                  <c:v>32</c:v>
+                </c:pt>
+                <c:pt idx="41">
+                  <c:v>64</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-AC5D-954F-802D-FA2688074A13}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet1!$C$1</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>N</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="25400" cap="rnd">
+              <a:noFill/>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent2"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="lt1"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:yVal>
+            <c:numRef>
+              <c:f>Sheet1!$C$2:$C$44</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="43"/>
+                <c:pt idx="0">
+                  <c:v>4096</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>4096</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>4096</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>4096</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>4096</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>4096</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>6144</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>6144</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>6144</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>6144</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>6144</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>6144</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>8192</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>8192</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>8192</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>8192</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>8192</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>8192</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>10240</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>10240</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>10240</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>10240</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>10240</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>10240</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>12288</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>12288</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>12288</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>12288</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>12288</c:v>
+                </c:pt>
+                <c:pt idx="29">
+                  <c:v>12288</c:v>
+                </c:pt>
+                <c:pt idx="30">
+                  <c:v>14336</c:v>
+                </c:pt>
+                <c:pt idx="31">
+                  <c:v>14336</c:v>
+                </c:pt>
+                <c:pt idx="32">
+                  <c:v>14336</c:v>
+                </c:pt>
+                <c:pt idx="33">
+                  <c:v>14336</c:v>
+                </c:pt>
+                <c:pt idx="34">
+                  <c:v>14336</c:v>
+                </c:pt>
+                <c:pt idx="35">
+                  <c:v>14336</c:v>
+                </c:pt>
+                <c:pt idx="36">
+                  <c:v>16384</c:v>
+                </c:pt>
+                <c:pt idx="37">
+                  <c:v>16384</c:v>
+                </c:pt>
+                <c:pt idx="38">
+                  <c:v>16384</c:v>
+                </c:pt>
+                <c:pt idx="39">
+                  <c:v>16384</c:v>
+                </c:pt>
+                <c:pt idx="40">
+                  <c:v>16384</c:v>
+                </c:pt>
+                <c:pt idx="41">
+                  <c:v>16384</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000001-AC5D-954F-802D-FA2688074A13}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="2"/>
+          <c:order val="2"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet1!$D$1</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>tid</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="25400" cap="rnd">
+              <a:noFill/>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent3"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="lt1"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:yVal>
+            <c:numRef>
+              <c:f>Sheet1!$D$2:$D$44</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="43"/>
+                <c:pt idx="0">
+                  <c:v>959</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>912</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>1142</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>1667</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>3083</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>4577</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>1498</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>1420</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>1810</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>2701</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>4746</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>7741</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>2061</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>1965</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>2531</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>3770</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>6408</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>10945</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>2664</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>2568</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>3251</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>4904</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>8068</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>14141</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>3257</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>3106</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>3967</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>5898</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>9732</c:v>
+                </c:pt>
+                <c:pt idx="29">
+                  <c:v>17339</c:v>
+                </c:pt>
+                <c:pt idx="30">
+                  <c:v>3864</c:v>
+                </c:pt>
+                <c:pt idx="31">
+                  <c:v>3687</c:v>
+                </c:pt>
+                <c:pt idx="32">
+                  <c:v>4683</c:v>
+                </c:pt>
+                <c:pt idx="33">
+                  <c:v>6956</c:v>
+                </c:pt>
+                <c:pt idx="34">
+                  <c:v>11393</c:v>
+                </c:pt>
+                <c:pt idx="35">
+                  <c:v>20521</c:v>
+                </c:pt>
+                <c:pt idx="36">
+                  <c:v>4479</c:v>
+                </c:pt>
+                <c:pt idx="37">
+                  <c:v>4240</c:v>
+                </c:pt>
+                <c:pt idx="38">
+                  <c:v>5400</c:v>
+                </c:pt>
+                <c:pt idx="39">
+                  <c:v>8018</c:v>
+                </c:pt>
+                <c:pt idx="40">
+                  <c:v>13052</c:v>
+                </c:pt>
+                <c:pt idx="41">
+                  <c:v>23726</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000002-AC5D-954F-802D-FA2688074A13}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:axId val="54375903"/>
+        <c:axId val="54377551"/>
+      </c:scatterChart>
+      <c:valAx>
+        <c:axId val="54375903"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="15000"/>
+                <a:lumOff val="85000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-DK"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="54377551"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:valAx>
+        <c:axId val="54377551"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-DK"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="54375903"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:extLst>
+      <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
+        <c16r3:dataDisplayOptions16>
+          <c16r3:dispNaAsBlank val="1"/>
+        </c16r3:dataDisplayOptions16>
+      </c:ext>
+    </c:extLst>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="en-DK"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/colors1.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
+<file path=xl/charts/style1.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="366">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+    </cs:spPr>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+    </cs:spPr>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="28575" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="lt1"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="28575" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="65000"/>
+          <a:lumOff val="35000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="75000"/>
+            <a:lumOff val="25000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat">
+        <a:solidFill>
+          <a:srgbClr val="D9D9D9"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDash"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>438150</xdr:colOff>
+      <xdr:row>3</xdr:row>
+      <xdr:rowOff>50800</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>12</xdr:col>
+      <xdr:colOff>457200</xdr:colOff>
+      <xdr:row>30</xdr:row>
+      <xdr:rowOff>76200</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="5" name="Chart 4">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{905264C2-D7D3-ED8D-3D6F-0EF5598F3A92}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/pivotCache/pivotCacheDefinition1.xml><?xml version="1.0" encoding="utf-8"?>
+<pivotCacheDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" r:id="rId1" refreshedBy="Microsoft Office User" refreshedDate="44950.71773113426" createdVersion="8" refreshedVersion="8" minRefreshableVersion="3" recordCount="42" xr:uid="{FA7A57F8-7F72-904E-A613-8A91F7763AF5}">
+  <cacheSource type="worksheet">
+    <worksheetSource ref="B1:D43" sheet="Sheet1"/>
+  </cacheSource>
+  <cacheFields count="3">
+    <cacheField name="K" numFmtId="0">
+      <sharedItems containsSemiMixedTypes="0" containsString="0" containsNumber="1" containsInteger="1" minValue="2" maxValue="64" count="6">
+        <n v="2"/>
+        <n v="4"/>
+        <n v="8"/>
+        <n v="16"/>
+        <n v="32"/>
+        <n v="64"/>
+      </sharedItems>
+    </cacheField>
+    <cacheField name="N" numFmtId="0">
+      <sharedItems containsSemiMixedTypes="0" containsString="0" containsNumber="1" containsInteger="1" minValue="4096" maxValue="16384" count="7">
+        <n v="4096"/>
+        <n v="6144"/>
+        <n v="8192"/>
+        <n v="10240"/>
+        <n v="12288"/>
+        <n v="14336"/>
+        <n v="16384"/>
+      </sharedItems>
+    </cacheField>
+    <cacheField name="tid" numFmtId="0">
+      <sharedItems containsSemiMixedTypes="0" containsString="0" containsNumber="1" containsInteger="1" minValue="912" maxValue="23726"/>
+    </cacheField>
+  </cacheFields>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{725AE2AE-9491-48be-B2B4-4EB974FC3084}">
+      <x14:pivotCacheDefinition/>
+    </ext>
+  </extLst>
+</pivotCacheDefinition>
+</file>
+
+<file path=xl/pivotCache/pivotCacheRecords1.xml><?xml version="1.0" encoding="utf-8"?>
+<pivotCacheRecords xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" count="42">
+  <r>
+    <x v="0"/>
+    <x v="0"/>
+    <n v="959"/>
+  </r>
+  <r>
+    <x v="1"/>
+    <x v="0"/>
+    <n v="912"/>
+  </r>
+  <r>
+    <x v="2"/>
+    <x v="0"/>
+    <n v="1142"/>
+  </r>
+  <r>
+    <x v="3"/>
+    <x v="0"/>
+    <n v="1667"/>
+  </r>
+  <r>
+    <x v="4"/>
+    <x v="0"/>
+    <n v="3083"/>
+  </r>
+  <r>
+    <x v="5"/>
+    <x v="0"/>
+    <n v="4577"/>
+  </r>
+  <r>
+    <x v="0"/>
+    <x v="1"/>
+    <n v="1498"/>
+  </r>
+  <r>
+    <x v="1"/>
+    <x v="1"/>
+    <n v="1420"/>
+  </r>
+  <r>
+    <x v="2"/>
+    <x v="1"/>
+    <n v="1810"/>
+  </r>
+  <r>
+    <x v="3"/>
+    <x v="1"/>
+    <n v="2701"/>
+  </r>
+  <r>
+    <x v="4"/>
+    <x v="1"/>
+    <n v="4746"/>
+  </r>
+  <r>
+    <x v="5"/>
+    <x v="1"/>
+    <n v="7741"/>
+  </r>
+  <r>
+    <x v="0"/>
+    <x v="2"/>
+    <n v="2061"/>
+  </r>
+  <r>
+    <x v="1"/>
+    <x v="2"/>
+    <n v="1965"/>
+  </r>
+  <r>
+    <x v="2"/>
+    <x v="2"/>
+    <n v="2531"/>
+  </r>
+  <r>
+    <x v="3"/>
+    <x v="2"/>
+    <n v="3770"/>
+  </r>
+  <r>
+    <x v="4"/>
+    <x v="2"/>
+    <n v="6408"/>
+  </r>
+  <r>
+    <x v="5"/>
+    <x v="2"/>
+    <n v="10945"/>
+  </r>
+  <r>
+    <x v="0"/>
+    <x v="3"/>
+    <n v="2664"/>
+  </r>
+  <r>
+    <x v="1"/>
+    <x v="3"/>
+    <n v="2568"/>
+  </r>
+  <r>
+    <x v="2"/>
+    <x v="3"/>
+    <n v="3251"/>
+  </r>
+  <r>
+    <x v="3"/>
+    <x v="3"/>
+    <n v="4904"/>
+  </r>
+  <r>
+    <x v="4"/>
+    <x v="3"/>
+    <n v="8068"/>
+  </r>
+  <r>
+    <x v="5"/>
+    <x v="3"/>
+    <n v="14141"/>
+  </r>
+  <r>
+    <x v="0"/>
+    <x v="4"/>
+    <n v="3257"/>
+  </r>
+  <r>
+    <x v="1"/>
+    <x v="4"/>
+    <n v="3106"/>
+  </r>
+  <r>
+    <x v="2"/>
+    <x v="4"/>
+    <n v="3967"/>
+  </r>
+  <r>
+    <x v="3"/>
+    <x v="4"/>
+    <n v="5898"/>
+  </r>
+  <r>
+    <x v="4"/>
+    <x v="4"/>
+    <n v="9732"/>
+  </r>
+  <r>
+    <x v="5"/>
+    <x v="4"/>
+    <n v="17339"/>
+  </r>
+  <r>
+    <x v="0"/>
+    <x v="5"/>
+    <n v="3864"/>
+  </r>
+  <r>
+    <x v="1"/>
+    <x v="5"/>
+    <n v="3687"/>
+  </r>
+  <r>
+    <x v="2"/>
+    <x v="5"/>
+    <n v="4683"/>
+  </r>
+  <r>
+    <x v="3"/>
+    <x v="5"/>
+    <n v="6956"/>
+  </r>
+  <r>
+    <x v="4"/>
+    <x v="5"/>
+    <n v="11393"/>
+  </r>
+  <r>
+    <x v="5"/>
+    <x v="5"/>
+    <n v="20521"/>
+  </r>
+  <r>
+    <x v="0"/>
+    <x v="6"/>
+    <n v="4479"/>
+  </r>
+  <r>
+    <x v="1"/>
+    <x v="6"/>
+    <n v="4240"/>
+  </r>
+  <r>
+    <x v="2"/>
+    <x v="6"/>
+    <n v="5400"/>
+  </r>
+  <r>
+    <x v="3"/>
+    <x v="6"/>
+    <n v="8018"/>
+  </r>
+  <r>
+    <x v="4"/>
+    <x v="6"/>
+    <n v="13052"/>
+  </r>
+  <r>
+    <x v="5"/>
+    <x v="6"/>
+    <n v="23726"/>
+  </r>
+</pivotCacheRecords>
+</file>
+
+<file path=xl/pivotTables/pivotTable1.xml><?xml version="1.0" encoding="utf-8"?>
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{0EA25067-58EB-A248-B0F1-E1134E4EF73B}" name="PivotTable1" cacheId="3" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="8" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
+  <location ref="A3:I11" firstHeaderRow="1" firstDataRow="2" firstDataCol="1"/>
+  <pivotFields count="3">
+    <pivotField axis="axisRow" showAll="0">
+      <items count="7">
+        <item x="0"/>
+        <item x="1"/>
+        <item x="2"/>
+        <item x="3"/>
+        <item x="4"/>
+        <item x="5"/>
+        <item t="default"/>
+      </items>
+    </pivotField>
+    <pivotField axis="axisCol" showAll="0">
+      <items count="8">
+        <item x="0"/>
+        <item x="1"/>
+        <item x="2"/>
+        <item x="3"/>
+        <item x="4"/>
+        <item x="5"/>
+        <item x="6"/>
+        <item t="default"/>
+      </items>
+    </pivotField>
+    <pivotField dataField="1" showAll="0"/>
+  </pivotFields>
+  <rowFields count="1">
+    <field x="0"/>
+  </rowFields>
+  <rowItems count="7">
+    <i>
+      <x/>
+    </i>
+    <i>
+      <x v="1"/>
+    </i>
+    <i>
+      <x v="2"/>
+    </i>
+    <i>
+      <x v="3"/>
+    </i>
+    <i>
+      <x v="4"/>
+    </i>
+    <i>
+      <x v="5"/>
+    </i>
+    <i t="grand">
+      <x/>
+    </i>
+  </rowItems>
+  <colFields count="1">
+    <field x="1"/>
+  </colFields>
+  <colItems count="8">
+    <i>
+      <x/>
+    </i>
+    <i>
+      <x v="1"/>
+    </i>
+    <i>
+      <x v="2"/>
+    </i>
+    <i>
+      <x v="3"/>
+    </i>
+    <i>
+      <x v="4"/>
+    </i>
+    <i>
+      <x v="5"/>
+    </i>
+    <i>
+      <x v="6"/>
+    </i>
+    <i t="grand">
+      <x/>
+    </i>
+  </colItems>
+  <dataFields count="1">
+    <dataField name="Sum of tid" fld="2" baseField="0" baseItem="0"/>
+  </dataFields>
+  <pivotTableStyleInfo name="PivotStyleLight16" showRowHeaders="1" showColHeaders="1" showRowStripes="0" showColStripes="0" showLastColumn="1"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{962EF5D1-5CA2-4c93-8EF4-DBF5C05439D2}">
+      <x14:pivotTableDefinition xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" hideValuesRow="1"/>
+    </ext>
+    <ext xmlns:xpdl="http://schemas.microsoft.com/office/spreadsheetml/2016/pivotdefaultlayout" uri="{747A6164-185A-40DC-8AA5-F01512510D54}">
+      <xpdl:pivotTableDefinition16/>
+    </ext>
+  </extLst>
+</pivotTableDefinition>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -525,11 +2282,271 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BA665A26-FA22-EE49-ACD0-C4EC7A69DE8E}">
+  <dimension ref="A3:I11"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A3" sqref="A3"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="13" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="15.5" bestFit="1" customWidth="1"/>
+    <col min="3" max="8" width="6.1640625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A3" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="B3" s="2" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A4" s="2" t="s">
+        <v>47</v>
+      </c>
+      <c r="B4">
+        <v>4096</v>
+      </c>
+      <c r="C4">
+        <v>6144</v>
+      </c>
+      <c r="D4">
+        <v>8192</v>
+      </c>
+      <c r="E4">
+        <v>10240</v>
+      </c>
+      <c r="F4">
+        <v>12288</v>
+      </c>
+      <c r="G4">
+        <v>14336</v>
+      </c>
+      <c r="H4">
+        <v>16384</v>
+      </c>
+      <c r="I4" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A5" s="3">
+        <v>2</v>
+      </c>
+      <c r="B5" s="4">
+        <v>959</v>
+      </c>
+      <c r="C5" s="4">
+        <v>1498</v>
+      </c>
+      <c r="D5" s="4">
+        <v>2061</v>
+      </c>
+      <c r="E5" s="4">
+        <v>2664</v>
+      </c>
+      <c r="F5" s="4">
+        <v>3257</v>
+      </c>
+      <c r="G5" s="4">
+        <v>3864</v>
+      </c>
+      <c r="H5" s="4">
+        <v>4479</v>
+      </c>
+      <c r="I5" s="4">
+        <v>18782</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A6" s="3">
+        <v>4</v>
+      </c>
+      <c r="B6" s="4">
+        <v>912</v>
+      </c>
+      <c r="C6" s="4">
+        <v>1420</v>
+      </c>
+      <c r="D6" s="4">
+        <v>1965</v>
+      </c>
+      <c r="E6" s="4">
+        <v>2568</v>
+      </c>
+      <c r="F6" s="4">
+        <v>3106</v>
+      </c>
+      <c r="G6" s="4">
+        <v>3687</v>
+      </c>
+      <c r="H6" s="4">
+        <v>4240</v>
+      </c>
+      <c r="I6" s="4">
+        <v>17898</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A7" s="3">
+        <v>8</v>
+      </c>
+      <c r="B7" s="4">
+        <v>1142</v>
+      </c>
+      <c r="C7" s="4">
+        <v>1810</v>
+      </c>
+      <c r="D7" s="4">
+        <v>2531</v>
+      </c>
+      <c r="E7" s="4">
+        <v>3251</v>
+      </c>
+      <c r="F7" s="4">
+        <v>3967</v>
+      </c>
+      <c r="G7" s="4">
+        <v>4683</v>
+      </c>
+      <c r="H7" s="4">
+        <v>5400</v>
+      </c>
+      <c r="I7" s="4">
+        <v>22784</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A8" s="3">
+        <v>16</v>
+      </c>
+      <c r="B8" s="4">
+        <v>1667</v>
+      </c>
+      <c r="C8" s="4">
+        <v>2701</v>
+      </c>
+      <c r="D8" s="4">
+        <v>3770</v>
+      </c>
+      <c r="E8" s="4">
+        <v>4904</v>
+      </c>
+      <c r="F8" s="4">
+        <v>5898</v>
+      </c>
+      <c r="G8" s="4">
+        <v>6956</v>
+      </c>
+      <c r="H8" s="4">
+        <v>8018</v>
+      </c>
+      <c r="I8" s="4">
+        <v>33914</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A9" s="3">
+        <v>32</v>
+      </c>
+      <c r="B9" s="4">
+        <v>3083</v>
+      </c>
+      <c r="C9" s="4">
+        <v>4746</v>
+      </c>
+      <c r="D9" s="4">
+        <v>6408</v>
+      </c>
+      <c r="E9" s="4">
+        <v>8068</v>
+      </c>
+      <c r="F9" s="4">
+        <v>9732</v>
+      </c>
+      <c r="G9" s="4">
+        <v>11393</v>
+      </c>
+      <c r="H9" s="4">
+        <v>13052</v>
+      </c>
+      <c r="I9" s="4">
+        <v>56482</v>
+      </c>
+    </row>
+    <row r="10" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A10" s="3">
+        <v>64</v>
+      </c>
+      <c r="B10" s="4">
+        <v>4577</v>
+      </c>
+      <c r="C10" s="4">
+        <v>7741</v>
+      </c>
+      <c r="D10" s="4">
+        <v>10945</v>
+      </c>
+      <c r="E10" s="4">
+        <v>14141</v>
+      </c>
+      <c r="F10" s="4">
+        <v>17339</v>
+      </c>
+      <c r="G10" s="4">
+        <v>20521</v>
+      </c>
+      <c r="H10" s="4">
+        <v>23726</v>
+      </c>
+      <c r="I10" s="4">
+        <v>98990</v>
+      </c>
+    </row>
+    <row r="11" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A11" s="3" t="s">
+        <v>48</v>
+      </c>
+      <c r="B11" s="4">
+        <v>12340</v>
+      </c>
+      <c r="C11" s="4">
+        <v>19916</v>
+      </c>
+      <c r="D11" s="4">
+        <v>27680</v>
+      </c>
+      <c r="E11" s="4">
+        <v>35596</v>
+      </c>
+      <c r="F11" s="4">
+        <v>43299</v>
+      </c>
+      <c r="G11" s="4">
+        <v>51104</v>
+      </c>
+      <c r="H11" s="4">
+        <v>58915</v>
+      </c>
+      <c r="I11" s="4">
+        <v>248850</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{71BAD5F0-C87B-FD4C-8641-43766FEDC887}">
   <dimension ref="A1:D43"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="C23" sqref="C23"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D5" sqref="D5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -544,596 +2561,604 @@
       <c r="C1" t="s">
         <v>43</v>
       </c>
+      <c r="D1" t="s">
+        <v>44</v>
+      </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A2" s="1" t="s">
-        <v>0</v>
+        <v>25</v>
       </c>
       <c r="B2" s="1">
-        <v>16</v>
+        <v>2</v>
       </c>
       <c r="C2" s="1">
-        <v>10240</v>
+        <v>4096</v>
       </c>
       <c r="D2">
-        <v>4904</v>
+        <v>959</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A3" s="1" t="s">
-        <v>1</v>
+        <v>27</v>
       </c>
       <c r="B3" s="1">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="C3" s="1">
-        <v>10240</v>
+        <v>4096</v>
       </c>
       <c r="D3">
-        <v>2664</v>
+        <v>912</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A4" s="1" t="s">
-        <v>2</v>
+        <v>29</v>
       </c>
       <c r="B4" s="1">
-        <v>32</v>
+        <v>8</v>
       </c>
       <c r="C4" s="1">
-        <v>10240</v>
+        <v>4096</v>
       </c>
       <c r="D4">
-        <v>8068</v>
+        <v>1142</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A5" s="1" t="s">
-        <v>3</v>
+        <v>24</v>
       </c>
       <c r="B5" s="1">
-        <v>4</v>
+        <v>16</v>
       </c>
       <c r="C5" s="1">
-        <v>10240</v>
+        <v>4096</v>
       </c>
       <c r="D5">
-        <v>2568</v>
+        <v>1667</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A6" s="1" t="s">
-        <v>4</v>
+        <v>26</v>
       </c>
       <c r="B6" s="1">
-        <v>64</v>
+        <v>32</v>
       </c>
       <c r="C6" s="1">
-        <v>10240</v>
+        <v>4096</v>
       </c>
       <c r="D6">
-        <v>14141</v>
+        <v>3083</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A7" s="1" t="s">
-        <v>5</v>
+        <v>28</v>
       </c>
       <c r="B7" s="1">
-        <v>8</v>
+        <v>64</v>
       </c>
       <c r="C7" s="1">
-        <v>10240</v>
+        <v>4096</v>
       </c>
       <c r="D7">
-        <v>3251</v>
+        <v>4577</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A8" s="1" t="s">
-        <v>6</v>
+        <v>31</v>
       </c>
       <c r="B8" s="1">
-        <v>16</v>
+        <v>2</v>
       </c>
       <c r="C8" s="1">
-        <v>12288</v>
+        <v>6144</v>
       </c>
       <c r="D8">
-        <v>5898</v>
+        <v>1498</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A9" s="1" t="s">
-        <v>7</v>
+        <v>33</v>
       </c>
       <c r="B9" s="1">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="C9" s="1">
-        <v>12288</v>
+        <v>6144</v>
       </c>
       <c r="D9">
-        <v>3257</v>
+        <v>1420</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A10" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="B10" s="1">
         <v>8</v>
       </c>
-      <c r="B10" s="1">
-        <v>32</v>
-      </c>
       <c r="C10" s="1">
-        <v>12288</v>
+        <v>6144</v>
       </c>
       <c r="D10">
-        <v>9732</v>
+        <v>1810</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A11" s="1" t="s">
-        <v>9</v>
+        <v>30</v>
       </c>
       <c r="B11" s="1">
-        <v>4</v>
+        <v>16</v>
       </c>
       <c r="C11" s="1">
-        <v>12288</v>
+        <v>6144</v>
       </c>
       <c r="D11">
-        <v>3106</v>
+        <v>2701</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A12" s="1" t="s">
-        <v>10</v>
+        <v>32</v>
       </c>
       <c r="B12" s="1">
-        <v>64</v>
+        <v>32</v>
       </c>
       <c r="C12" s="1">
-        <v>12288</v>
+        <v>6144</v>
       </c>
       <c r="D12">
-        <v>17339</v>
+        <v>4746</v>
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A13" s="1" t="s">
-        <v>11</v>
+        <v>34</v>
       </c>
       <c r="B13" s="1">
-        <v>8</v>
+        <v>64</v>
       </c>
       <c r="C13" s="1">
-        <v>12288</v>
+        <v>6144</v>
       </c>
       <c r="D13">
-        <v>3967</v>
+        <v>7741</v>
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A14" s="1" t="s">
-        <v>12</v>
+        <v>37</v>
       </c>
       <c r="B14" s="1">
-        <v>16</v>
+        <v>2</v>
       </c>
       <c r="C14" s="1">
-        <v>14336</v>
+        <v>8192</v>
       </c>
       <c r="D14">
-        <v>6956</v>
+        <v>2061</v>
       </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A15" s="1" t="s">
-        <v>13</v>
+        <v>39</v>
       </c>
       <c r="B15" s="1">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="C15" s="1">
-        <v>14336</v>
+        <v>8192</v>
       </c>
       <c r="D15">
-        <v>3864</v>
+        <v>1965</v>
       </c>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A16" s="1" t="s">
-        <v>14</v>
+        <v>41</v>
       </c>
       <c r="B16" s="1">
-        <v>32</v>
+        <v>8</v>
       </c>
       <c r="C16" s="1">
-        <v>14336</v>
+        <v>8192</v>
       </c>
       <c r="D16">
-        <v>11393</v>
+        <v>2531</v>
       </c>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A17" s="1" t="s">
-        <v>15</v>
+        <v>36</v>
       </c>
       <c r="B17" s="1">
-        <v>4</v>
+        <v>16</v>
       </c>
       <c r="C17" s="1">
-        <v>14336</v>
+        <v>8192</v>
       </c>
       <c r="D17">
-        <v>3687</v>
+        <v>3770</v>
       </c>
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A18" s="1" t="s">
-        <v>16</v>
+        <v>38</v>
       </c>
       <c r="B18" s="1">
-        <v>64</v>
+        <v>32</v>
       </c>
       <c r="C18" s="1">
-        <v>14336</v>
+        <v>8192</v>
       </c>
       <c r="D18">
-        <v>20521</v>
+        <v>6408</v>
       </c>
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A19" s="1" t="s">
-        <v>17</v>
+        <v>40</v>
       </c>
       <c r="B19" s="1">
-        <v>8</v>
+        <v>64</v>
       </c>
       <c r="C19" s="1">
-        <v>14336</v>
+        <v>8192</v>
       </c>
       <c r="D19">
-        <v>4683</v>
+        <v>10945</v>
       </c>
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A20" s="1" t="s">
-        <v>18</v>
+        <v>1</v>
       </c>
       <c r="B20" s="1">
-        <v>16</v>
+        <v>2</v>
       </c>
       <c r="C20" s="1">
-        <v>16384</v>
+        <v>10240</v>
       </c>
       <c r="D20">
-        <v>8018</v>
+        <v>2664</v>
       </c>
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A21" s="1" t="s">
-        <v>19</v>
+        <v>3</v>
       </c>
       <c r="B21" s="1">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="C21" s="1">
-        <v>16384</v>
+        <v>10240</v>
       </c>
       <c r="D21">
-        <v>4479</v>
+        <v>2568</v>
       </c>
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A22" s="1" t="s">
-        <v>20</v>
+        <v>5</v>
       </c>
       <c r="B22" s="1">
-        <v>32</v>
+        <v>8</v>
       </c>
       <c r="C22" s="1">
-        <v>16384</v>
+        <v>10240</v>
       </c>
       <c r="D22">
-        <v>13052</v>
+        <v>3251</v>
       </c>
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A23" s="1" t="s">
-        <v>21</v>
+        <v>0</v>
       </c>
       <c r="B23" s="1">
-        <v>4</v>
+        <v>16</v>
       </c>
       <c r="C23" s="1">
-        <v>16384</v>
+        <v>10240</v>
       </c>
       <c r="D23">
-        <v>4240</v>
+        <v>4904</v>
       </c>
     </row>
     <row r="24" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A24" s="1" t="s">
-        <v>22</v>
+        <v>2</v>
       </c>
       <c r="B24" s="1">
-        <v>64</v>
+        <v>32</v>
       </c>
       <c r="C24" s="1">
-        <v>16384</v>
+        <v>10240</v>
       </c>
       <c r="D24">
-        <v>23726</v>
+        <v>8068</v>
       </c>
     </row>
     <row r="25" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A25" s="1" t="s">
-        <v>23</v>
+        <v>4</v>
       </c>
       <c r="B25" s="1">
-        <v>8</v>
+        <v>64</v>
       </c>
       <c r="C25" s="1">
-        <v>16384</v>
+        <v>10240</v>
       </c>
       <c r="D25">
-        <v>5400</v>
+        <v>14141</v>
       </c>
     </row>
     <row r="26" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A26" s="1" t="s">
-        <v>24</v>
+        <v>7</v>
       </c>
       <c r="B26" s="1">
-        <v>16</v>
+        <v>2</v>
       </c>
       <c r="C26" s="1">
-        <v>4096</v>
+        <v>12288</v>
       </c>
       <c r="D26">
-        <v>1667</v>
+        <v>3257</v>
       </c>
     </row>
     <row r="27" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A27" s="1" t="s">
-        <v>25</v>
+        <v>9</v>
       </c>
       <c r="B27" s="1">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="C27" s="1">
-        <v>4096</v>
+        <v>12288</v>
       </c>
       <c r="D27">
-        <v>959</v>
+        <v>3106</v>
       </c>
     </row>
     <row r="28" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A28" s="1" t="s">
-        <v>26</v>
+        <v>11</v>
       </c>
       <c r="B28" s="1">
-        <v>32</v>
+        <v>8</v>
       </c>
       <c r="C28" s="1">
-        <v>4096</v>
+        <v>12288</v>
       </c>
       <c r="D28">
-        <v>3083</v>
+        <v>3967</v>
       </c>
     </row>
     <row r="29" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A29" s="1" t="s">
-        <v>27</v>
+        <v>6</v>
       </c>
       <c r="B29" s="1">
-        <v>4</v>
+        <v>16</v>
       </c>
       <c r="C29" s="1">
-        <v>4096</v>
+        <v>12288</v>
       </c>
       <c r="D29">
-        <v>912</v>
+        <v>5898</v>
       </c>
     </row>
     <row r="30" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A30" s="1" t="s">
-        <v>28</v>
+        <v>8</v>
       </c>
       <c r="B30" s="1">
-        <v>64</v>
+        <v>32</v>
       </c>
       <c r="C30" s="1">
-        <v>4096</v>
+        <v>12288</v>
       </c>
       <c r="D30">
-        <v>4577</v>
+        <v>9732</v>
       </c>
     </row>
     <row r="31" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A31" s="1" t="s">
-        <v>29</v>
+        <v>10</v>
       </c>
       <c r="B31" s="1">
-        <v>8</v>
+        <v>64</v>
       </c>
       <c r="C31" s="1">
-        <v>4096</v>
+        <v>12288</v>
       </c>
       <c r="D31">
-        <v>1142</v>
+        <v>17339</v>
       </c>
     </row>
     <row r="32" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A32" s="1" t="s">
-        <v>30</v>
+        <v>13</v>
       </c>
       <c r="B32" s="1">
-        <v>16</v>
+        <v>2</v>
       </c>
       <c r="C32" s="1">
-        <v>6144</v>
+        <v>14336</v>
       </c>
       <c r="D32">
-        <v>2701</v>
+        <v>3864</v>
       </c>
     </row>
     <row r="33" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A33" s="1" t="s">
-        <v>31</v>
+        <v>15</v>
       </c>
       <c r="B33" s="1">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="C33" s="1">
-        <v>6144</v>
+        <v>14336</v>
       </c>
       <c r="D33">
-        <v>1498</v>
+        <v>3687</v>
       </c>
     </row>
     <row r="34" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A34" s="1" t="s">
-        <v>32</v>
+        <v>17</v>
       </c>
       <c r="B34" s="1">
-        <v>32</v>
+        <v>8</v>
       </c>
       <c r="C34" s="1">
-        <v>6144</v>
+        <v>14336</v>
       </c>
       <c r="D34">
-        <v>4746</v>
+        <v>4683</v>
       </c>
     </row>
     <row r="35" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A35" s="1" t="s">
-        <v>33</v>
+        <v>12</v>
       </c>
       <c r="B35" s="1">
-        <v>4</v>
+        <v>16</v>
       </c>
       <c r="C35" s="1">
-        <v>6144</v>
+        <v>14336</v>
       </c>
       <c r="D35">
-        <v>1420</v>
+        <v>6956</v>
       </c>
     </row>
     <row r="36" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A36" s="1" t="s">
-        <v>34</v>
+        <v>14</v>
       </c>
       <c r="B36" s="1">
-        <v>64</v>
+        <v>32</v>
       </c>
       <c r="C36" s="1">
-        <v>6144</v>
+        <v>14336</v>
       </c>
       <c r="D36">
-        <v>7741</v>
+        <v>11393</v>
       </c>
     </row>
     <row r="37" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A37" s="1" t="s">
-        <v>35</v>
+        <v>16</v>
       </c>
       <c r="B37" s="1">
-        <v>8</v>
+        <v>64</v>
       </c>
       <c r="C37" s="1">
-        <v>6144</v>
+        <v>14336</v>
       </c>
       <c r="D37">
-        <v>1810</v>
+        <v>20521</v>
       </c>
     </row>
     <row r="38" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A38" s="1" t="s">
-        <v>36</v>
+        <v>19</v>
       </c>
       <c r="B38" s="1">
-        <v>16</v>
+        <v>2</v>
       </c>
       <c r="C38" s="1">
-        <v>8192</v>
+        <v>16384</v>
       </c>
       <c r="D38">
-        <v>3770</v>
+        <v>4479</v>
       </c>
     </row>
     <row r="39" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A39" s="1" t="s">
-        <v>37</v>
+        <v>21</v>
       </c>
       <c r="B39" s="1">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="C39" s="1">
-        <v>8192</v>
+        <v>16384</v>
       </c>
       <c r="D39">
-        <v>2061</v>
+        <v>4240</v>
       </c>
     </row>
     <row r="40" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A40" s="1" t="s">
-        <v>38</v>
+        <v>23</v>
       </c>
       <c r="B40" s="1">
-        <v>32</v>
+        <v>8</v>
       </c>
       <c r="C40" s="1">
-        <v>8192</v>
+        <v>16384</v>
       </c>
       <c r="D40">
-        <v>6408</v>
+        <v>5400</v>
       </c>
     </row>
     <row r="41" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A41" s="1" t="s">
-        <v>39</v>
+        <v>18</v>
       </c>
       <c r="B41" s="1">
-        <v>4</v>
+        <v>16</v>
       </c>
       <c r="C41" s="1">
-        <v>8192</v>
+        <v>16384</v>
       </c>
       <c r="D41">
-        <v>1965</v>
+        <v>8018</v>
       </c>
     </row>
     <row r="42" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A42" s="1" t="s">
-        <v>40</v>
+        <v>20</v>
       </c>
       <c r="B42" s="1">
-        <v>64</v>
+        <v>32</v>
       </c>
       <c r="C42" s="1">
-        <v>8192</v>
+        <v>16384</v>
       </c>
       <c r="D42">
-        <v>10945</v>
+        <v>13052</v>
       </c>
     </row>
     <row r="43" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A43" s="1" t="s">
-        <v>41</v>
+        <v>22</v>
       </c>
       <c r="B43" s="1">
-        <v>8</v>
+        <v>64</v>
       </c>
       <c r="C43" s="1">
-        <v>8192</v>
+        <v>16384</v>
       </c>
       <c r="D43">
-        <v>2531</v>
+        <v>23726</v>
       </c>
     </row>
   </sheetData>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:D43">
+    <sortCondition ref="C2:C43"/>
+    <sortCondition ref="B2:B43"/>
+  </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>